<commit_message>
Add Motobike Page & Update requirement = discount, remark
</commit_message>
<xml_diff>
--- a/static/templates/booking_template.xlsx
+++ b/static/templates/booking_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00.Work_Freelance\Tour\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38E715D-AD1B-42EC-9CFF-0F3145011343}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAF71A0-F35E-4646-A314-AA1086C07911}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928" xr2:uid="{1F82F821-8D6E-7643-BBAF-FED4C6234257}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8925" xr2:uid="{1F82F821-8D6E-7643-BBAF-FED4C6234257}"/>
   </bookViews>
   <sheets>
     <sheet name="Tour &amp; Motorbike rental" sheetId="1" r:id="rId1"/>
@@ -23,23 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
   <si>
     <t>BOOKING CONFIRMATION</t>
   </si>
@@ -89,9 +78,6 @@
     <t>TEL : +66 77 420 789    E-MAIL : info@lamaibayviewboutique.co.th</t>
   </si>
   <si>
-    <t>PAYMENT</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -132,6 +118,18 @@
   </si>
   <si>
     <t>Travel date</t>
+  </si>
+  <si>
+    <t>REMARK</t>
+  </si>
+  <si>
+    <t>PAYMENT METHOD</t>
+  </si>
+  <si>
+    <t>PAYMET METHOD</t>
+  </si>
+  <si>
+    <t>STATUS</t>
   </si>
 </sst>
 </file>
@@ -405,44 +403,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
@@ -459,13 +421,49 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -906,46 +904,46 @@
   </sheetPr>
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A43" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="24.6"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="25.5"/>
   <cols>
-    <col min="1" max="1" width="1.26953125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="1.26953125" style="2" customWidth="1"/>
-    <col min="4" max="7" width="10.7265625" style="2"/>
-    <col min="8" max="8" width="16.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.81640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="1.26953125" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="10.7265625" style="2"/>
+    <col min="1" max="1" width="1.21875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="1.21875" style="2" customWidth="1"/>
+    <col min="4" max="7" width="10.77734375" style="2"/>
+    <col min="8" max="8" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="1.21875" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="10.77734375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="J1" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="27">
-      <c r="A2" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="26.25">
+      <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
     </row>
     <row r="3" spans="1:11">
       <c r="I3" s="9"/>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -953,18 +951,18 @@
       <c r="I4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="6" customHeight="1"/>
-    <row r="6" spans="1:11" ht="16.05" customHeight="1">
+    <row r="6" spans="1:11" ht="16.149999999999999" customHeight="1">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="16.05" customHeight="1">
+    <row r="7" spans="1:11" ht="16.149999999999999" customHeight="1">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -974,7 +972,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="16.05" customHeight="1">
+    <row r="9" spans="1:11" ht="16.149999999999999" customHeight="1">
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
@@ -984,46 +982,46 @@
       <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>25</v>
+      <c r="D11" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:11" ht="7.95" customHeight="1"/>
+    <row r="12" spans="1:11" ht="7.9" customHeight="1"/>
     <row r="13" spans="1:11">
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="21" t="s">
-        <v>30</v>
+      <c r="F13" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I13" s="20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="7.95" customHeight="1"/>
+      <c r="I13" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="7.9" customHeight="1"/>
     <row r="15" spans="1:11">
       <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="17"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="32"/>
       <c r="H15" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>13</v>
@@ -1033,52 +1031,52 @@
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="B16" s="34"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
-      <c r="D16" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="30"/>
+      <c r="D16" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="17"/>
+      <c r="J16" s="18"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="B17" s="34"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="30"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="18"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="B18" s="34"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="30"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="18"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="B19" s="35"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="33"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="21"/>
     </row>
     <row r="20" spans="1:11">
       <c r="B20" s="5"/>
@@ -1087,44 +1085,51 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="19"/>
-      <c r="J20" s="36">
+      <c r="I20" s="36"/>
+      <c r="J20" s="24">
         <f>SUM(K6:K19)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="10.050000000000001" customHeight="1"/>
-    <row r="22" spans="1:11" s="20" customFormat="1">
-      <c r="B22" s="20" t="s">
+    <row r="21" spans="1:11" ht="24.6" customHeight="1">
+      <c r="B21" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="14" customFormat="1">
+      <c r="B22" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="F22" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="14" customFormat="1"/>
+    <row r="24" spans="1:11" s="14" customFormat="1">
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="14" customFormat="1">
+      <c r="B25" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="14" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="20" customFormat="1"/>
-    <row r="24" spans="1:11" s="20" customFormat="1">
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" s="20" customFormat="1">
-      <c r="B25" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1142,27 +1147,27 @@
     </row>
     <row r="28" spans="1:11">
       <c r="J28" s="13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="27">
-      <c r="A29" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="26.25">
+      <c r="A29" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
     </row>
     <row r="30" spans="1:11">
       <c r="I30" s="9"/>
-      <c r="J30" s="20" t="s">
+      <c r="J30" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1170,18 +1175,18 @@
       <c r="I31" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J31" s="20" t="s">
+      <c r="J31" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="6" customHeight="1"/>
-    <row r="33" spans="2:10" ht="16.05" customHeight="1">
+    <row r="33" spans="2:10" ht="16.149999999999999" customHeight="1">
       <c r="B33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="2:10" ht="16.05" customHeight="1">
+    <row r="34" spans="2:10" ht="16.149999999999999" customHeight="1">
       <c r="B34" s="1" t="s">
         <v>7</v>
       </c>
@@ -1191,53 +1196,53 @@
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="2:10" ht="16.05" customHeight="1">
+    <row r="36" spans="2:10" ht="16.149999999999999" customHeight="1">
       <c r="B36" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C36" s="1"/>
     </row>
-    <row r="38" spans="2:10" s="20" customFormat="1">
-      <c r="B38" s="20" t="s">
+    <row r="38" spans="2:10" s="14" customFormat="1">
+      <c r="B38" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" s="20" customFormat="1" ht="7.95" customHeight="1"/>
-    <row r="40" spans="2:10" s="20" customFormat="1">
-      <c r="B40" s="20" t="s">
+      <c r="D38" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" s="14" customFormat="1" ht="7.9" customHeight="1"/>
+    <row r="40" spans="2:10" s="14" customFormat="1">
+      <c r="B40" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D40" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="37" t="s">
+      <c r="E40" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F40" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="H40" s="37" t="s">
+      <c r="F40" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I40" s="20" t="s">
+      <c r="H40" s="25" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="41" spans="2:10" ht="7.95" customHeight="1"/>
+      <c r="I40" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" ht="7.9" customHeight="1"/>
     <row r="42" spans="2:10">
       <c r="B42" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="17"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="32"/>
       <c r="H42" s="12" t="s">
         <v>12</v>
       </c>
@@ -1248,99 +1253,107 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="2:10" s="20" customFormat="1">
-      <c r="B43" s="34"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="I43" s="29"/>
-      <c r="J43" s="30"/>
-    </row>
-    <row r="44" spans="2:10" s="20" customFormat="1">
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="30"/>
-    </row>
-    <row r="45" spans="2:10" s="20" customFormat="1">
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="30"/>
-    </row>
-    <row r="46" spans="2:10" s="20" customFormat="1">
-      <c r="B46" s="35"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="33"/>
-    </row>
-    <row r="47" spans="2:10" s="20" customFormat="1">
-      <c r="B47" s="39"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="40" t="s">
+    <row r="43" spans="2:10" s="14" customFormat="1">
+      <c r="B43" s="22"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I43" s="17"/>
+      <c r="J43" s="18"/>
+    </row>
+    <row r="44" spans="2:10" s="14" customFormat="1">
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="18"/>
+    </row>
+    <row r="45" spans="2:10" s="14" customFormat="1">
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="18"/>
+    </row>
+    <row r="46" spans="2:10" s="14" customFormat="1">
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="41"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="21"/>
+    </row>
+    <row r="47" spans="2:10" s="14" customFormat="1">
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="I47" s="41"/>
-      <c r="J47" s="36">
+      <c r="I47" s="34"/>
+      <c r="J47" s="24">
         <f>SUM(K33:K46)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:10" ht="10.050000000000001" customHeight="1"/>
-    <row r="49" spans="2:9" s="20" customFormat="1">
-      <c r="B49" s="20" t="s">
+    <row r="48" spans="2:10" ht="24.6" customHeight="1">
+      <c r="B48" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="14"/>
+    </row>
+    <row r="49" spans="2:9" s="14" customFormat="1">
+      <c r="B49" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D49" s="20" t="s">
+      <c r="F49" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" s="14" customFormat="1"/>
+    <row r="51" spans="2:9" s="14" customFormat="1">
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G51" s="28"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" s="14" customFormat="1">
+      <c r="B52" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G52" s="14" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" s="20" customFormat="1"/>
-    <row r="51" spans="2:9" s="20" customFormat="1">
-      <c r="B51" s="42"/>
-      <c r="C51" s="42"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="2:9" s="20" customFormat="1">
-      <c r="B52" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G52" s="20" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1355,7 +1368,7 @@
     <mergeCell ref="D43:G46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="65" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="61" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
print to pdf done all template
</commit_message>
<xml_diff>
--- a/static/templates/booking_template.xlsx
+++ b/static/templates/booking_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00.Work_Freelance\Tour\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B3C385-37FB-4F58-8C55-CC6E17C19E69}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDF6892-AB4B-477F-956A-66D7CEE760A2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8925" xr2:uid="{1F82F821-8D6E-7643-BBAF-FED4C6234257}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
   <si>
     <t>BOOKING CONFIRMATION</t>
   </si>
@@ -93,9 +93,6 @@
     <t>GUEST</t>
   </si>
   <si>
-    <t>List</t>
-  </si>
-  <si>
     <t>ORIGINAL</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>Price / Quantity</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
@@ -133,6 +127,9 @@
   </si>
   <si>
     <t>PAYMENT</t>
+  </si>
+  <si>
+    <t>DISCOUNT</t>
   </si>
 </sst>
 </file>
@@ -223,7 +220,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -298,19 +295,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -326,30 +310,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -376,12 +338,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -389,14 +362,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -408,30 +377,59 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -449,23 +447,11 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -907,8 +893,8 @@
   </sheetPr>
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="25.5"/>
@@ -926,36 +912,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="J1" s="13" t="s">
-        <v>22</v>
+      <c r="J1" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="26.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="I3" s="9"/>
-      <c r="J3" s="14" t="s">
+      <c r="I3" s="6"/>
+      <c r="J3" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -986,8 +972,8 @@
       <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>24</v>
+      <c r="D11" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="E11" s="3"/>
     </row>
@@ -996,20 +982,20 @@
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="14" t="s">
+      <c r="F13" s="11" t="s">
         <v>27</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="7.9" customHeight="1"/>
@@ -1017,15 +1003,15 @@
       <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="11" t="s">
-        <v>25</v>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>13</v>
@@ -1035,157 +1021,155 @@
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="B16" s="22"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="18"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="B17" s="22"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="18"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="B18" s="22"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="18"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="B19" s="23"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="21"/>
+      <c r="B19" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="35" t="s">
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="24">
+      <c r="I20" s="35"/>
+      <c r="J20" s="12">
         <f>SUM(J16:J19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="24.6" customHeight="1">
       <c r="B21" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="14" customFormat="1">
-      <c r="B22" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="10" customFormat="1">
+      <c r="B22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="14" customFormat="1"/>
-    <row r="24" spans="1:11" s="14" customFormat="1">
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="14" t="s">
+      <c r="F22" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="10" customFormat="1"/>
+    <row r="24" spans="1:11" s="10" customFormat="1">
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="14" t="s">
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="14" customFormat="1">
-      <c r="B25" s="14" t="s">
+    <row r="25" spans="1:11" s="10" customFormat="1">
+      <c r="B25" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="J28" s="13" t="s">
-        <v>23</v>
+      <c r="J28" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="26.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
     </row>
     <row r="30" spans="1:11">
-      <c r="I30" s="9"/>
-      <c r="J30" s="14" t="s">
+      <c r="I30" s="6"/>
+      <c r="J30" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:11">
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J31" s="14" t="s">
+      <c r="J31" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1212,33 +1196,33 @@
       </c>
       <c r="C36" s="1"/>
     </row>
-    <row r="38" spans="2:10" s="14" customFormat="1">
-      <c r="B38" s="14" t="s">
+    <row r="38" spans="2:10" s="10" customFormat="1">
+      <c r="B38" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" s="14" customFormat="1" ht="7.9" customHeight="1"/>
-    <row r="40" spans="2:10" s="14" customFormat="1">
-      <c r="B40" s="14" t="s">
+      <c r="D38" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" s="10" customFormat="1" ht="7.9" customHeight="1"/>
+    <row r="40" spans="2:10" s="10" customFormat="1">
+      <c r="B40" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="25" t="s">
+      <c r="E40" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F40" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H40" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I40" s="14" t="s">
+      <c r="F40" s="11" t="s">
         <v>27</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="2:10" ht="7.9" customHeight="1"/>
@@ -1246,14 +1230,14 @@
       <c r="B42" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="30" t="s">
+      <c r="C42" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="12" t="s">
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I42" s="4" t="s">
@@ -1263,111 +1247,109 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="2:10" s="14" customFormat="1">
-      <c r="B43" s="22"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="I43" s="17"/>
-      <c r="J43" s="18"/>
-    </row>
-    <row r="44" spans="2:10" s="14" customFormat="1">
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="16"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="18"/>
-    </row>
-    <row r="45" spans="2:10" s="14" customFormat="1">
-      <c r="B45" s="22"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="40"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="18"/>
-    </row>
-    <row r="46" spans="2:10" s="14" customFormat="1">
-      <c r="B46" s="23"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="21"/>
-    </row>
-    <row r="47" spans="2:10" s="14" customFormat="1">
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="33" t="s">
+    <row r="43" spans="2:10" s="10" customFormat="1">
+      <c r="B43" s="15"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="22"/>
+    </row>
+    <row r="44" spans="2:10" s="10" customFormat="1">
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="22"/>
+    </row>
+    <row r="45" spans="2:10" s="10" customFormat="1">
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="22"/>
+    </row>
+    <row r="46" spans="2:10" s="10" customFormat="1">
+      <c r="B46" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="24"/>
+    </row>
+    <row r="47" spans="2:10" s="10" customFormat="1">
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="I47" s="34"/>
-      <c r="J47" s="24">
+      <c r="I47" s="33"/>
+      <c r="J47" s="12">
         <f>SUM(J43:J46)</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="24.6" customHeight="1">
       <c r="B48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" s="10" customFormat="1">
+      <c r="B49" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" s="14" customFormat="1">
-      <c r="B49" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F49" s="14" t="s">
+      <c r="H49" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H49" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" s="14" customFormat="1"/>
-    <row r="51" spans="2:9" s="14" customFormat="1">
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="14" t="s">
+    </row>
+    <row r="50" spans="2:9" s="10" customFormat="1"/>
+    <row r="51" spans="2:9" s="10" customFormat="1">
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G51" s="28"/>
-      <c r="H51" s="28"/>
-      <c r="I51" s="14" t="s">
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="2:9" s="14" customFormat="1">
-      <c r="B52" s="14" t="s">
+    <row r="52" spans="2:9" s="10" customFormat="1">
+      <c r="B52" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G52" s="14" t="s">
+      <c r="G52" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1379,8 +1361,8 @@
     <mergeCell ref="H47:I47"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="C15:G15"/>
-    <mergeCell ref="D16:G19"/>
-    <mergeCell ref="D43:G46"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B46:I46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="59" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>